<commit_message>
Agregando la funcionalidads de apagar reiniciar el sistema
</commit_message>
<xml_diff>
--- a/static/download/admin/Reporte General de Ventas.xlsx
+++ b/static/download/admin/Reporte General de Ventas.xlsx
@@ -25,7 +25,7 @@
     <t>REPORTE DE VENTAS</t>
   </si>
   <si>
-    <t>DEL DIA 2014-10-13 0:00:00 AL DIA 2014-10-27 23:59:59</t>
+    <t>DEL DIA 2014-09-28 0:00:00 AL DIA 2014-10-27 23:59:59</t>
   </si>
   <si>
     <t>Tarifa</t>
@@ -587,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="4">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -598,10 +598,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="4">
-        <v>703</v>
+        <v>883</v>
       </c>
       <c r="E13" s="3">
-        <v>1406</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -609,10 +609,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="4">
-        <v>4094</v>
+        <v>4138</v>
       </c>
       <c r="E14" s="3">
-        <v>12282</v>
+        <v>12414</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -620,10 +620,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="4">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="E15" s="3">
-        <v>300</v>
+        <v>875</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="4">
-        <v>5004</v>
+        <v>5369</v>
       </c>
     </row>
     <row r="19" spans="3:4">
@@ -645,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="3">
-        <v>13989</v>
+        <v>15082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando nuevas imagenes al sistema
</commit_message>
<xml_diff>
--- a/static/download/admin/Reporte General de Ventas.xlsx
+++ b/static/download/admin/Reporte General de Ventas.xlsx
@@ -25,7 +25,7 @@
     <t>REPORTE DE VENTAS</t>
   </si>
   <si>
-    <t>DEL DIA 2014-10-21 0:00:00 AL DIA 2014-10-21 23:59:59</t>
+    <t>DEL DIA 2014-10-28 0:00:00 AL DIA 2014-10-28 23:59:59</t>
   </si>
   <si>
     <t>Tarifa</t>
@@ -573,35 +573,35 @@
     </row>
     <row r="11" spans="1:6">
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="C12" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="4">
-        <v>174</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3">
-        <v>522</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="C13" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>40</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -615,7 +615,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="4">
-        <v>197</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -623,7 +623,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="3">
-        <v>562</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>